<commit_message>
Modificacion data driven framework
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
-    <sheet name="DATA" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="LOGIN" sheetId="3" r:id="rId2"/>
+    <sheet name="HOTEL" sheetId="4" r:id="rId3"/>
+    <sheet name="URL" sheetId="5" r:id="rId4"/>
+    <sheet name="COUPON" sheetId="6" r:id="rId5"/>
+    <sheet name="DATA" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="46">
   <si>
     <t>TEST ID</t>
   </si>
@@ -45,9 +48,6 @@
     <t>lmmdpass</t>
   </si>
   <si>
-    <t>KEYWORDS</t>
-  </si>
-  <si>
     <t>USERNAME|PASSWORD</t>
   </si>
   <si>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t>URL|COUPON|NAME_H|LAST_H|EMAIL_H</t>
+  </si>
+  <si>
+    <t>BUSINESS FLOW</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -526,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +549,7 @@
     <col min="4" max="4" width="53.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,91 +560,175 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
       <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
         <v>37</v>
       </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -645,10 +738,172 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E3"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43678</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43692</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="L1" sqref="I1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,34 +929,34 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
       <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>22</v>
-      </c>
-      <c r="L1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -712,7 +967,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2">
         <v>43678</v>
@@ -727,16 +982,16 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>26</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -745,16 +1000,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Project POM clothes store
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -2,24 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
     <sheet name="LOGIN" sheetId="3" r:id="rId2"/>
-    <sheet name="HOTEL" sheetId="4" r:id="rId3"/>
-    <sheet name="URL" sheetId="5" r:id="rId4"/>
-    <sheet name="COUPON" sheetId="6" r:id="rId5"/>
-    <sheet name="DATA" sheetId="2" r:id="rId6"/>
+    <sheet name="ITEM" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>TEST ID</t>
   </si>
@@ -42,33 +39,9 @@
     <t>T3</t>
   </si>
   <si>
-    <t>lmmd@lmmd.com</t>
-  </si>
-  <si>
-    <t>lmmdpass</t>
-  </si>
-  <si>
     <t>USERNAME|PASSWORD</t>
   </si>
   <si>
-    <t>HOTEL</t>
-  </si>
-  <si>
-    <t>CHECKIN</t>
-  </si>
-  <si>
-    <t>CHECKOUT</t>
-  </si>
-  <si>
-    <t>Singapore</t>
-  </si>
-  <si>
-    <t>NUM_ADULTS</t>
-  </si>
-  <si>
-    <t>NUM_CHILDS</t>
-  </si>
-  <si>
     <t>T2</t>
   </si>
   <si>
@@ -78,82 +51,79 @@
     <t>Access to website with valid credentials</t>
   </si>
   <si>
-    <t>COUPON</t>
-  </si>
-  <si>
-    <t>NAME_H</t>
-  </si>
-  <si>
-    <t>LAST_H</t>
-  </si>
-  <si>
-    <t>EMAIL_H</t>
-  </si>
-  <si>
-    <t>ElRw</t>
-  </si>
-  <si>
-    <t>Axel</t>
-  </si>
-  <si>
-    <t>Trl</t>
-  </si>
-  <si>
-    <t>axeltrl@gmail.com</t>
-  </si>
-  <si>
-    <t>SEARCH HOTEL</t>
-  </si>
-  <si>
     <t>T4</t>
   </si>
   <si>
-    <t>CHECK AMENITIES</t>
-  </si>
-  <si>
     <t>T5</t>
   </si>
   <si>
-    <t>VERIFY CHECKING INFORMATION</t>
-  </si>
-  <si>
     <t>T6</t>
   </si>
   <si>
-    <t>BOOK HOTEL</t>
-  </si>
-  <si>
-    <t>Given some search criteria, found certain hotel</t>
-  </si>
-  <si>
-    <t>According to found hotel, verify the availability</t>
-  </si>
-  <si>
-    <t>VERIFY AVAILABILITY</t>
-  </si>
-  <si>
-    <t>According to found hotel, verify the amenities</t>
-  </si>
-  <si>
-    <t>According to found hotel, verify the checking information</t>
-  </si>
-  <si>
-    <t>Book the desired hotel</t>
-  </si>
-  <si>
-    <t>HOTEL|CHECKIN|CHECKOUT|NUM_ADULTS|NUM_CHILDS</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>URL|COUPON|NAME_H|LAST_H|EMAIL_H</t>
-  </si>
-  <si>
     <t>BUSINESS FLOW</t>
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>SEARCH ITEM</t>
+  </si>
+  <si>
+    <t>CHOOSE ITEM</t>
+  </si>
+  <si>
+    <t>CHECK ADDRESS</t>
+  </si>
+  <si>
+    <t>CHECK SHIPPING</t>
+  </si>
+  <si>
+    <t>futbol01</t>
+  </si>
+  <si>
+    <t>black_panther_xaa@hotmail.com</t>
+  </si>
+  <si>
+    <t>Given some search criteria like name, found certain item</t>
+  </si>
+  <si>
+    <t>Choose the found item</t>
+  </si>
+  <si>
+    <t>Fill and verify address to ship</t>
+  </si>
+  <si>
+    <t>CONFIRM ORDER</t>
+  </si>
+  <si>
+    <t>Fill and verify shipping carrier</t>
+  </si>
+  <si>
+    <t>Confirm the order</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>Blouse</t>
+  </si>
+  <si>
+    <t>QUANTITY</t>
+  </si>
+  <si>
+    <t>SIZE</t>
+  </si>
+  <si>
+    <t>COLOR</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>ITEM|QUANTITY|SIZE|COLOR</t>
   </si>
   <si>
     <t>-</t>
@@ -535,10 +505,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +520,7 @@
     <col min="4" max="4" width="53.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -560,175 +531,121 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -738,15 +655,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:E3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -760,10 +678,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -778,226 +696,49 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="D2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2">
-        <v>43678</v>
-      </c>
-      <c r="C2" s="2">
-        <v>43692</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="I1:L2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2">
-        <v>43678</v>
-      </c>
-      <c r="E2" s="2">
-        <v>43692</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Creacion de pdf con imagenes
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
-    <sheet name="LOGIN" sheetId="3" r:id="rId2"/>
+    <sheet name="LOGIN" sheetId="8" r:id="rId2"/>
     <sheet name="ITEM" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -171,10 +171,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -509,7 +508,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,11 +654,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:E3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,27 +666,25 @@
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>3</v>
       </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correcciones en excel y en busqueda de articulo
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
-    <sheet name="LOGIN" sheetId="8" r:id="rId2"/>
+    <sheet name="LOGIN" sheetId="3" r:id="rId2"/>
     <sheet name="ITEM" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>TEST ID</t>
   </si>
@@ -39,9 +39,6 @@
     <t>T3</t>
   </si>
   <si>
-    <t>USERNAME|PASSWORD</t>
-  </si>
-  <si>
     <t>T2</t>
   </si>
   <si>
@@ -123,10 +120,13 @@
     <t>White</t>
   </si>
   <si>
-    <t>ITEM|QUANTITY|SIZE|COLOR</t>
-  </si>
-  <si>
-    <t>-</t>
+    <t>login</t>
+  </si>
+  <si>
+    <t>addItem</t>
+  </si>
+  <si>
+    <t>completeOrder</t>
   </si>
 </sst>
 </file>
@@ -171,9 +171,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -504,11 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,13 +530,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -544,39 +544,33 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -584,67 +578,46 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -654,10 +627,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A2:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,25 +639,27 @@
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -692,11 +667,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="D2:I3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,30 +682,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
         <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>